<commit_message>
Added outsourcing to simulation
</commit_message>
<xml_diff>
--- a/ProcessDiagramsCharts/ResourceStaffingChart.xlsx
+++ b/ProcessDiagramsCharts/ResourceStaffingChart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>Resource Staffing Chart</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Without Error</t>
+  </si>
+  <si>
+    <t>Updated with New Resources</t>
   </si>
 </sst>
 </file>
@@ -88,17 +91,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -207,11 +214,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2122504312"/>
-        <c:axId val="-2122335944"/>
+        <c:axId val="-2141241224"/>
+        <c:axId val="-2141236712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2122504312"/>
+        <c:axId val="-2141241224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -239,7 +246,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122335944"/>
+        <c:crossAx val="-2141236712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -247,7 +254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122335944"/>
+        <c:axId val="-2141236712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -277,7 +284,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122504312"/>
+        <c:crossAx val="-2141241224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -394,11 +401,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2121989400"/>
-        <c:axId val="-2121990392"/>
+        <c:axId val="-2141823176"/>
+        <c:axId val="-2141828632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2121989400"/>
+        <c:axId val="-2141823176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +433,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121990392"/>
+        <c:crossAx val="-2141828632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -434,7 +441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121990392"/>
+        <c:axId val="-2141828632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -469,7 +476,383 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121989400"/>
+        <c:crossAx val="-2141823176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Resource Staffing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart (w/ Error)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$52:$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Designers</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Implementers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Testers</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Managers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$52:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2123584952"/>
+        <c:axId val="2120678408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2123584952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Employee Type</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2120678408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2120678408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># of People</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2123584952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Resource Staffing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart (w/o Error)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$52:$C$55</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Designers</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Implementers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Testers</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Managers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$52:$D$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2068127176"/>
+        <c:axId val="-2137810760"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2068127176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Employee Type</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2137810760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2137810760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># of People</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2068127176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -543,6 +926,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -873,15 +1316,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -952,6 +1395,75 @@
       </c>
       <c r="D6">
         <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Resource Staffing Chart with Outsource Data
</commit_message>
<xml_diff>
--- a/ProcessDiagramsCharts/ResourceStaffingChart.xlsx
+++ b/ProcessDiagramsCharts/ResourceStaffingChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="0" windowWidth="33160" windowHeight="20980" tabRatio="500"/>
+    <workbookView xWindow="14420" yWindow="0" windowWidth="24080" windowHeight="20980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Resource Staffing Chart</t>
   </si>
@@ -42,7 +42,13 @@
     <t>Without Error</t>
   </si>
   <si>
-    <t>Updated with New Resources</t>
+    <t>Updated with New Resources and Outsourcing</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Offshore</t>
   </si>
 </sst>
 </file>
@@ -91,8 +97,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -101,11 +111,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -518,13 +532,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Resource Staffing</a:t>
+              <a:t>Resource Staffing Chart (w/o Error)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Chart (w/ Error)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -541,6 +550,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Local</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -569,13 +589,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0</c:v>
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Offshore</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$52:$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Designers</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Implementers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Testers</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Managers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$52:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.0</c:v>
@@ -594,11 +671,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2123584952"/>
-        <c:axId val="2120678408"/>
+        <c:axId val="-2125342232"/>
+        <c:axId val="-2125340824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2123584952"/>
+        <c:axId val="-2125342232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,7 +703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120678408"/>
+        <c:crossAx val="-2125340824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -634,7 +711,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2120678408"/>
+        <c:axId val="-2125340824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,11 +741,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123584952"/>
+        <c:crossAx val="-2125342232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -706,11 +788,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Resource Staffing</a:t>
+              <a:t>Resource</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Chart (w/o Error)</a:t>
+              <a:t> Staffing Chart (w/ Error)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -729,10 +811,21 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Local</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$52:$C$55</c:f>
+              <c:f>Sheet1!$D$52:$D$55</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -752,18 +845,75 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$52:$D$55</c:f>
+              <c:f>Sheet1!$E$52:$E$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0</c:v>
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Offshore</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$52:$D$55</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Designers</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Implementers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Testers</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Managers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$52:$F$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.0</c:v>
@@ -782,11 +932,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2068127176"/>
-        <c:axId val="-2137810760"/>
+        <c:axId val="-2133194280"/>
+        <c:axId val="-2131203864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2068127176"/>
+        <c:axId val="-2133194280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,7 +964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137810760"/>
+        <c:crossAx val="-2131203864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -822,7 +972,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2137810760"/>
+        <c:axId val="-2131203864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,7 +990,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t># of People</a:t>
+                  <a:t># of people</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -852,11 +1002,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2068127176"/>
+        <c:crossAx val="-2133194280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -934,19 +1089,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -965,18 +1120,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="8" name="Chart 7"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1316,16 +1471,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1397,72 +1552,102 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>1</v>
+    <row r="51" spans="1:6">
+      <c r="B51" t="s">
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>2</v>
       </c>
       <c r="B52">
-        <v>8</v>
-      </c>
-      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
         <v>2</v>
       </c>
-      <c r="D52">
-        <v>8</v>
+      <c r="E52">
+        <v>6</v>
+      </c>
+      <c r="F52">
+        <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>4</v>
       </c>
       <c r="B53">
-        <v>8</v>
-      </c>
-      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
         <v>4</v>
       </c>
-      <c r="D53">
-        <v>8</v>
+      <c r="E53">
+        <v>6</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>5</v>
       </c>
       <c r="B54">
-        <v>8</v>
-      </c>
-      <c r="C54" t="s">
         <v>5</v>
       </c>
-      <c r="D54">
-        <v>8</v>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54">
+        <v>6</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>3</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
         <v>3</v>
       </c>
-      <c r="D55">
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
         <v>1</v>
       </c>
     </row>

</xml_diff>